<commit_message>
Alterado arquivo de resultados do modelo GPT-2
</commit_message>
<xml_diff>
--- a/Abordagens/GPT-2/Resultados/suggestions_2_word.xlsx
+++ b/Abordagens/GPT-2/Resultados/suggestions_2_word.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Organizado\Acadêmicos\Usp\Pós Graduação\Monografia\Repo\TCC.SugestoesCodigo.Pece.IA\Abordagens\GPT-2\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9C281F-F261-43E8-A355-FB0FE72A7424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B1460F-D4A0-4102-843B-EF9E0E3000A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19280" yWindow="10" windowWidth="19360" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suggestions_2_word" sheetId="1" r:id="rId1"/>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -1336,7 +1336,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5">
         <f>(G4*100)/G3</f>
-        <v>30.357142857142858</v>
+        <v>30.90909090909091</v>
       </c>
       <c r="H5" s="5"/>
     </row>
@@ -1376,7 +1376,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5">
         <f>(G6*100)/G3</f>
-        <v>67.857142857142861</v>
+        <v>69.090909090909093</v>
       </c>
       <c r="H7" s="5"/>
     </row>

</xml_diff>